<commit_message>
fixing NaExceptions in the integration tests
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it-graph/src/test/resources/standard_excel_files/Isna_Fx.xlsx
+++ b/calculation-engine/engine-tests/engine-it-graph/src/test/resources/standard_excel_files/Isna_Fx.xlsx
@@ -426,9 +426,21 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D6" t="e">
-        <f ca="1">INDEX(9, _xlfn.SHEET(2))</f>
-        <v>#N/A</v>
+      <c r="D6" t="str">
+        <f>INDEX(A1:B5,1,2)</f>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7">
+        <f>2+3</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D8">
+        <f>3+2</f>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -452,6 +464,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000BBA6CFB0E2DE4B9D0F8FC00657BC00" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b5fa52e5d42efb553dd3c6ab2e94e30b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -565,12 +583,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{702E4E43-5E1B-45FB-B00E-49F0F864E71D}">
   <ds:schemaRefs>
@@ -580,6 +592,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BCCFA4A-4F32-4E75-B993-8AA6FB6449E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1922868A-8AA3-46E7-93AD-114661C8621F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -593,13 +614,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BCCFA4A-4F32-4E75-B993-8AA6FB6449E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixing converting issues for Name and NA errors
</commit_message>
<xml_diff>
--- a/calculation-engine/engine-tests/engine-it-graph/src/test/resources/standard_excel_files/Isna_Fx.xlsx
+++ b/calculation-engine/engine-tests/engine-it-graph/src/test/resources/standard_excel_files/Isna_Fx.xlsx
@@ -426,21 +426,9 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D6" t="str">
-        <f>INDEX(A1:B5,1,2)</f>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D7">
-        <f>2+3</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D8">
-        <f>3+2</f>
-        <v>5</v>
+      <c r="D6" t="e">
+        <f ca="1">INDEX(9, _xlfn.SHEET(2))</f>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -464,12 +452,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010000BBA6CFB0E2DE4B9D0F8FC00657BC00" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="b5fa52e5d42efb553dd3c6ab2e94e30b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -583,6 +565,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{702E4E43-5E1B-45FB-B00E-49F0F864E71D}">
   <ds:schemaRefs>
@@ -592,15 +580,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BCCFA4A-4F32-4E75-B993-8AA6FB6449E5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1922868A-8AA3-46E7-93AD-114661C8621F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -614,4 +593,13 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BCCFA4A-4F32-4E75-B993-8AA6FB6449E5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>